<commit_message>
Ajout capteur ultrason + servo
</commit_message>
<xml_diff>
--- a/doc/Idées/Biblio/Annexe - liste de composants.xlsx
+++ b/doc/Idées/Biblio/Annexe - liste de composants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\etude\S5\Projet\Snoopytech\doc\Idées\Biblio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6F9841-7A97-4B4E-B76D-2D031E2B41AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57611FF9-D36D-42D9-9B84-2FCD9FEA9918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3560E6F7-E16C-476D-B8B1-12EB76F63514}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Moteurs</t>
   </si>
@@ -102,6 +102,33 @@
   </si>
   <si>
     <t>Tube en fibre de carbone brillant 3K</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/Scanradius-LIDAR-Sensorscanner-Vermeidung-Hindernissen-Navigation/dp/B07VLFGT27/ref=asc_df_B07VLFGT27/?tag=googshopfr-21&amp;linkCode=df0&amp;hvadid=411439987151&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17858514273165735039&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9054956&amp;hvtargid=pla-843524520219&amp;psc=1&amp;tag=&amp;ref=&amp;adgrpid=95238321811&amp;hvpone=&amp;hvptwo=&amp;hvadid=411439987151&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17858514273165735039&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9054956&amp;hvtargid=pla-843524520219</t>
+  </si>
+  <si>
+    <t>Lidar</t>
+  </si>
+  <si>
+    <t>youyeetoo Slamtec RPLIDAR</t>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/32880359778.html?spm=a2g0o.productlist.0.0.57cd4b01vpsFWo&amp;algo_pvid=1dd6e5ce-0655-4592-a3d3-c60e37e11f4e&amp;algo_exp_id=1dd6e5ce-0655-4592-a3d3-c60e37e11f4e-8&amp;pdp_ext_f=%7B%22sku_id%22%3A%2265583297495%22%7D&amp;pdp_npi=2%40dis%21EUR%211.27%211.23%21%21%21%21%21%402100bddd16651281964884006e0ba3%2165583297495%21sea&amp;curPageLogUid=97KgxLHc40fl</t>
+  </si>
+  <si>
+    <t>Capteur</t>
+  </si>
+  <si>
+    <t>Capteur ultrason</t>
+  </si>
+  <si>
+    <t>MG90S SG90 9g – avion télécommandé Miniature, équipement de direction à ailes fixes, modèle d'avion 250 450, hélicoptère, voiture jouet | AliExpress</t>
+  </si>
+  <si>
+    <t>Servo SG90</t>
+  </si>
+  <si>
+    <t>Servo</t>
   </si>
 </sst>
 </file>
@@ -149,7 +176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -160,6 +187,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -478,7 +506,7 @@
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +616,7 @@
       <c r="G5" s="1">
         <v>5</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -616,7 +644,7 @@
       <c r="G6" s="1">
         <v>71</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -624,24 +652,84 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>109.99</v>
+      </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>109.99</v>
+      </c>
+      <c r="G7" s="1">
+        <v>363</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.23</v>
+      </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.23</v>
+      </c>
+      <c r="G8" s="1">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="2"/>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.9</v>
+      </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9</v>
+      </c>
+      <c r="G9" s="1">
+        <v>9</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -721,8 +809,13 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1" xr:uid="{04A81B08-ED2E-4B28-942B-ACF961888121}"/>
+    <hyperlink ref="H8" r:id="rId2" display="https://fr.aliexpress.com/item/32880359778.html?spm=a2g0o.productlist.0.0.57cd4b01vpsFWo&amp;algo_pvid=1dd6e5ce-0655-4592-a3d3-c60e37e11f4e&amp;algo_exp_id=1dd6e5ce-0655-4592-a3d3-c60e37e11f4e-8&amp;pdp_ext_f=%7B%22sku_id%22%3A%2265583297495%22%7D&amp;pdp_npi=2%40dis%21EUR%211.27%211.23%21%21%21%21%21%402100bddd16651281964884006e0ba3%2165583297495%21sea&amp;curPageLogUid=97KgxLHc40fl" xr:uid="{A08DFE88-9A6B-407E-8EE2-7A8699A25427}"/>
+    <hyperlink ref="H7" r:id="rId3" display="https://www.amazon.fr/Scanradius-LIDAR-Sensorscanner-Vermeidung-Hindernissen-Navigation/dp/B07VLFGT27/ref=asc_df_B07VLFGT27/?tag=googshopfr-21&amp;linkCode=df0&amp;hvadid=411439987151&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17858514273165735039&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9054956&amp;hvtargid=pla-843524520219&amp;psc=1&amp;tag=&amp;ref=&amp;adgrpid=95238321811&amp;hvpone=&amp;hvptwo=&amp;hvadid=411439987151&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17858514273165735039&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9054956&amp;hvtargid=pla-843524520219" xr:uid="{59B75DE9-FFB1-4E5B-8133-126D03E53BEB}"/>
+    <hyperlink ref="H6" r:id="rId4" display="https://fr.aliexpress.com/item/1005002248466483.html?spm=a2g0o.productlist.0.0.26b421abnfmSYq&amp;algo_pvid=47e13833-caa3-437f-9553-01e57919688d&amp;algo_exp_id=47e13833-caa3-437f-9553-01e57919688d-45&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000019728171207%22%7D&amp;pdp_npi=2%40dis%21EUR%218.39%217.14%21%21%214.99%21%21%400b0a050b16651254583308408eed58%2112000019728171207%21sea&amp;curPageLogUid=nz516Ros1nuv" xr:uid="{9FC859F5-FCB4-423E-AD9C-C5ACA81E0215}"/>
+    <hyperlink ref="H5" r:id="rId5" display="https://fr.aliexpress.com/item/32997948364.html?algo_pvid=f64572da-108a-4531-a5a0-b856b462b1c6&amp;algo_exp_id=f64572da-108a-4531-a5a0-b856b462b1c6-7&amp;pdp_ext_f=%7B%22sku_id%22%3A%2266958865882%22%7D&amp;pdp_npi=2%40dis%21EUR%210.95%210.95%21%21%212.76%21%21%400b0a187b16651255256126173ec49c%2166958865882%21sea&amp;curPageLogUid=OfDWACxdeGQE" xr:uid="{C5EAE7AA-BF47-4AFF-949F-11FFA21234D8}"/>
+    <hyperlink ref="H9" r:id="rId6" display="https://fr.aliexpress.com/item/32807449919.html?spm=a2g0o.productlist.0.0.26ba6ddfwD1PpD&amp;algo_pvid=2c2733ee-cc9e-4061-ba5d-445e38ffbc8f&amp;algo_exp_id=2c2733ee-cc9e-4061-ba5d-445e38ffbc8f-2&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000029113111881%22%7D&amp;pdp_npi=2%40dis%21EUR%212.46%210.24%21%21%211.77%21%21%402100bde316651285671751244ed3c5%2112000029113111881%21sea&amp;curPageLogUid=s9Hmx7xeBNxQ" xr:uid="{EFC63950-DF96-40E0-ACBF-9E536741EE0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update liste de composant
</commit_message>
<xml_diff>
--- a/doc/Idées/Biblio/Annexe - liste de composants.xlsx
+++ b/doc/Idées/Biblio/Annexe - liste de composants.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t xml:space="preserve">Nom</t>
   </si>
@@ -122,6 +122,27 @@
   </si>
   <si>
     <t xml:space="preserve">https://fr.aliexpress.com/item/1005003187542470.html?gps-id=pcDetailBottomMoreOtherSeller&amp;scm=1007.40050.281175.0&amp;scm_id=1007.40050.281175.0&amp;scm-url=1007.40050.281175.0&amp;pvid=c304510e-3a7a-4b7f-a621-847c700dce94&amp;_t=gps-id:pcDetailBottomMoreOtherSeller,scm-url:1007.40050.281175.0,pvid:c304510e-3a7a-4b7f-a621-847c700dce94,tpp_buckets:668%232846%238115%232000&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000024565611228%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=2%40dis%21EUR%217.75%216.28%21%21%21%21%21%40211b58ee16651293083523082e1a4c%2112000024565611228%21rec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potentiometre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potentiometre 10K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fr.aliexpress.com/item/32996236826.html?spm=a2g0o.detail.1000060.3.2dfd75067cm24G&amp;gps-id=pcDetailBottomMoreThisSeller&amp;scm=1007.13339.291025.0&amp;scm_id=1007.13339.291025.0&amp;scm-url=1007.13339.291025.0&amp;pvid=aa5bbdd6-37f4-4697-8922-a5d47906774f&amp;_t=gps-id%3ApcDetailBottomMoreThisSeller%2Cscm-url%3A1007.13339.291025.0%2Cpvid%3Aaa5bbdd6-37f4-4697-8922-a5d47906774f%2Ctpp_buckets%3A668%232846%238116%232002&amp;pdp_ext_f=%7B%22sku_id%22%3A%2266994016160%22%2C%22sceneId%22%3A%223339%22%7D&amp;pdp_npi=2%40dis%21EUR%210.77%210.68%21%21%21%21%21%402103222316652351797365094e1aae%2166994016160%21rec&amp;gatewayAdapt=glo2fra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color: 10 K Ohm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accelerometre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPU6050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fr.aliexpress.com/item/32340949017.html?spm=a2g0o.productlist.0.0.587312adnNgBZj&amp;algo_pvid=19376db7-79d4-41f3-91f8-c1871eddb2a7&amp;algo_exp_id=19376db7-79d4-41f3-91f8-c1871eddb2a7-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2210000000609322940%22%7D&amp;pdp_npi=2%40dis%21EUR%211.62%211.42%21%21%211.71%21%21%402101e9d416652354615517308e70c3%2110000000609322940%21sea&amp;curPageLogUid=c2sYDhCk9WsN</t>
   </si>
 </sst>
 </file>
@@ -311,7 +332,7 @@
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -565,18 +586,59 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="2"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.68</v>
+      </c>
       <c r="F11" s="2" t="n">
-        <f aca="false">E11*D11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="2"/>
+        <f aca="false">E11*D11+0.99</f>
+        <v>2.35</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <f aca="false">1.42+1.17</f>
+        <v>2.59</v>
+      </c>
       <c r="F12" s="2" t="n">
         <f aca="false">E12*D12</f>
-        <v>0</v>
+        <v>2.59</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,6 +702,8 @@
     <hyperlink ref="H7" r:id="rId4" display="https://www.amazon.fr/Scanradius-LIDAR-Sensorscanner-Vermeidung-Hindernissen-Navigation/dp/B07VLFGT27/ref=asc_df_B07VLFGT27/?tag=googshopfr-21&amp;linkCode=df0&amp;hvadid=411439987151&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17858514273165735039&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9054956&amp;hvtargid=pla-843524520219&amp;psc=1&amp;tag=&amp;ref=&amp;adgrpid=95238321811&amp;hvpone=&amp;hvptwo=&amp;hvadid=411439987151&amp;hvpos=&amp;hvnetw=g&amp;hvrand=17858514273165735039&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9054956&amp;hvtargid=pla-843524520219"/>
     <hyperlink ref="H8" r:id="rId5" display="https://fr.aliexpress.com/item/32880359778.html?spm=a2g0o.productlist.0.0.57cd4b01vpsFWo&amp;algo_pvid=1dd6e5ce-0655-4592-a3d3-c60e37e11f4e&amp;algo_exp_id=1dd6e5ce-0655-4592-a3d3-c60e37e11f4e-8&amp;pdp_ext_f=%7B%22sku_id%22%3A%2265583297495%22%7D&amp;pdp_npi=2%40dis%21EUR%211.27%211.23%21%21%21%21%21%402100bddd16651281964884006e0ba3%2165583297495%21sea&amp;curPageLogUid=97KgxLHc40fl"/>
     <hyperlink ref="H9" r:id="rId6" display="MG90S SG90 9g – avion télécommandé Miniature, équipement de direction à ailes fixes, modèle d'avion 250 450, hélicoptère, voiture jouet | AliExpress"/>
+    <hyperlink ref="H11" r:id="rId7" display="https://fr.aliexpress.com/item/32996236826.html?spm=a2g0o.detail.1000060.3.2dfd75067cm24G&amp;gps-id=pcDetailBottomMoreThisSeller&amp;scm=1007.13339.291025.0&amp;scm_id=1007.13339.291025.0&amp;scm-url=1007.13339.291025.0&amp;pvid=aa5bbdd6-37f4-4697-8922-a5d47906774f&amp;_t=gps-id%3ApcDetailBottomMoreThisSeller%2Cscm-url%3A1007.13339.291025.0%2Cpvid%3Aaa5bbdd6-37f4-4697-8922-a5d47906774f%2Ctpp_buckets%3A668%232846%238116%232002&amp;pdp_ext_f=%7B%22sku_id%22%3A%2266994016160%22%2C%22sceneId%22%3A%223339%22%7D&amp;pdp_npi=2%40dis%21EUR%210.77%210.68%21%21%21%21%21%402103222316652351797365094e1aae%2166994016160%21rec&amp;gatewayAdapt=glo2fra"/>
+    <hyperlink ref="H12" r:id="rId8" display="https://fr.aliexpress.com/item/32340949017.html?spm=a2g0o.productlist.0.0.587312adnNgBZj&amp;algo_pvid=19376db7-79d4-41f3-91f8-c1871eddb2a7&amp;algo_exp_id=19376db7-79d4-41f3-91f8-c1871eddb2a7-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2210000000609322940%22%7D&amp;pdp_npi=2%40dis%21EUR%211.62%211.42%21%21%211.71%21%21%402101e9d416652354615517308e70c3%2110000000609322940%21sea&amp;curPageLogUid=c2sYDhCk9WsN"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
2nd report - week 42
</commit_message>
<xml_diff>
--- a/doc/Idées/Biblio/Annexe - liste de composants.xlsx
+++ b/doc/Idées/Biblio/Annexe - liste de composants.xlsx
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Potentiometre 10K</t>
   </si>
   <si>
-    <t xml:space="preserve">https://fr.aliexpress.com/item/1005001421294754.html?spm=a2g0o.detail.1000014.14.6d93d6c1kfyDHn&amp;gps-id=pcDetailBottomMoreOtherSeller&amp;scm=1007.40050.281175.0&amp;scm_id=1007.40050.281175.0&amp;scm-url=1007.40050.281175.0&amp;pvid=0c4a9003-02ec-45be-823d-ab61eb9fdcb9&amp;_t=gps-id:pcDetailBottomMoreOtherSeller,scm-url:1007.40050.281175.0,pvid:0c4a9003-02ec-45be-823d-ab61eb9fdcb9,tpp_buckets:668%232846%238116%232002&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000016052827770%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=2%40dis%21EUR%210.64%210.5%21%21%21%21%21%402101f6b416658298845222455e1af7%2112000016052827770%21rec</t>
+    <t xml:space="preserve">https://fr.aliexpress.com/item/1005002766893077.html?spm=a2g0o.detail.1000014.28.6d93d6c1fPOoi0&amp;gps-id=pcDetailBottomMoreOtherSeller&amp;scm=1007.40050.281175.0&amp;scm_id=1007.40050.281175.0&amp;scm-url=1007.40050.281175.0&amp;pvid=c4eb49e9-017c-42e1-bc5a-36d0b91caa96&amp;_t=gps-id:pcDetailBottomMoreOtherSeller,scm-url:1007.40050.281175.0,pvid:c4eb49e9-017c-42e1-bc5a-36d0b91caa96,tpp_buckets:668%232846%238116%232002&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000022084500624%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=2%40dis%21EUR%210.42%210.37%21%21%21%21%21%402101f6b416658300092574280e1af7%2112000022084500624%21rec</t>
   </si>
   <si>
     <t xml:space="preserve">Color: 10 K Ohm</t>
@@ -473,7 +473,7 @@
   <dimension ref="C1:J32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -747,11 +747,11 @@
         <v>3</v>
       </c>
       <c r="E15" s="18" t="n">
-        <v>0.51</v>
+        <v>0.37</v>
       </c>
       <c r="F15" s="18" t="n">
-        <f aca="false">E15*D15+2</f>
-        <v>3.53</v>
+        <f aca="false">E15*D15+0.99</f>
+        <v>2.1</v>
       </c>
       <c r="G15" s="17" t="n">
         <v>10</v>
@@ -794,7 +794,7 @@
       </c>
       <c r="D17" s="24" t="n">
         <f aca="false">SUM(F5:F16)</f>
-        <v>580.28</v>
+        <v>578.85</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>34</v>
@@ -1003,7 +1003,7 @@
     <hyperlink ref="H12" r:id="rId6" display="https://fr.aliexpress.com/item/32880359778.html?spm=a2g0o.productlist.0.0.57cd4b01vpsFWo&amp;algo_pvid=1dd6e5ce-0655-4592-a3d3-c60e37e11f4e&amp;algo_exp_id=1dd6e5ce-0655-4592-a3d3-c60e37e11f4e-8&amp;pdp_ext_f=%7B%22sku_id%22%3A%2265583297495%22%7D&amp;pdp_npi=2%40dis%21EUR%211.27%211.23%21%21%21%21%21%402100bddd16651281964884006e0ba3%2165583297495%21sea&amp;curPageLogUid=97KgxLHc40fl"/>
     <hyperlink ref="H13" r:id="rId7" display="MG90S SG90 9g – avion télécommandé Miniature, équipement de direction à ailes fixes, modèle d'avion 250 450, hélicoptère, voiture jouet | AliExpress"/>
     <hyperlink ref="H14" r:id="rId8" display="https://fr.aliexpress.com/item/1005003187542470.html?gps-id=pcDetailBottomMoreOtherSeller&amp;scm=1007.40050.281175.0&amp;scm_id=1007.40050.281175.0&amp;scm-url=1007.40050.281175.0&amp;pvid=c304510e-3a7a-4b7f-a621-847c700dce94&amp;_t=gps-id:pcDetailBottomMoreOtherSeller,scm-url:1007.40050.281175.0,pvid:c304510e-3a7a-4b7f-a621-847c700dce94,tpp_buckets:668%232846%238115%232000&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000024565611228%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=2%40dis%21EUR%217.75%216.28%21%21%21%21%21%40211b58ee16651293083523082e1a4c%2112000024565611228%21rec/"/>
-    <hyperlink ref="H15" r:id="rId9" display="https://fr.aliexpress.com/item/1005001421294754.html?spm=a2g0o.detail.1000014.14.6d93d6c1kfyDHn&amp;gps-id=pcDetailBottomMoreOtherSeller&amp;scm=1007.40050.281175.0&amp;scm_id=1007.40050.281175.0&amp;scm-url=1007.40050.281175.0&amp;pvid=0c4a9003-02ec-45be-823d-ab61eb9fdcb9&amp;_t=gps-id:pcDetailBottomMoreOtherSeller,scm-url:1007.40050.281175.0,pvid:0c4a9003-02ec-45be-823d-ab61eb9fdcb9,tpp_buckets:668%232846%238116%232002&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000016052827770%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=2%40dis%21EUR%210.64%210.5%21%21%21%21%21%402101f6b416658298845222455e1af7%2112000016052827770%21rec"/>
+    <hyperlink ref="H15" r:id="rId9" display="https://fr.aliexpress.com/item/1005002766893077.html?spm=a2g0o.detail.1000014.28.6d93d6c1fPOoi0&amp;gps-id=pcDetailBottomMoreOtherSeller&amp;scm=1007.40050.281175.0&amp;scm_id=1007.40050.281175.0&amp;scm-url=1007.40050.281175.0&amp;pvid=c4eb49e9-017c-42e1-bc5a-36d0b91caa96&amp;_t=gps-id:pcDetailBottomMoreOtherSeller,scm-url:1007.40050.281175.0,pvid:c4eb49e9-017c-42e1-bc5a-36d0b91caa96,tpp_buckets:668%232846%238116%232002&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000022084500624%22%2C%22sceneId%22%3A%2230050%22%7D&amp;pdp_npi=2%40dis%21EUR%210.42%210.37%21%21%21%21%21%402101f6b416658300092574280e1af7%2112000022084500624%21rec"/>
     <hyperlink ref="H16" r:id="rId10" display="https://fr.aliexpress.com/item/32340949017.html?spm=a2g0o.productlist.0.0.587312adnNgBZj&amp;algo_pvid=19376db7-79d4-41f3-91f8-c1871eddb2a7&amp;algo_exp_id=19376db7-79d4-41f3-91f8-c1871eddb2a7-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2210000000609322940%22%7D&amp;pdp_npi=2%40dis%21EUR%211.62%211.42%21%21%211.71%21%21%402101e9d416652354615517308e70c3%2110000000609322940%21sea&amp;curPageLogUid=c2sYDhCk9WsN"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>